<commit_message>
Deploying to gh-pages from  @ 6752f3c9cce58723b51673caa3fcdfe4afe78340 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_5-1-2.xlsx
+++ b/assets/excel/2021_5-1-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring_2021\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC12D90-DE88-4536-A33E-D70DB47355C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA59CA0C-9353-49B5-97C1-D06E9B697413}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11205" xr2:uid="{85247E4B-3EF4-475F-BA74-B7C111865EC2}"/>
   </bookViews>
@@ -139,11 +139,17 @@
     <t>https://www.integrationsmonitoring.niedersachsen.de</t>
   </si>
   <si>
-    <t>Indikator 5.2.1: Erwerbsquote, Erwerbstätigenquote und Erwerbslosenanteil nach Zuwanderungsgeschichte</t>
+    <t xml:space="preserve">4) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes: </t>
+  </si>
+  <si>
+    <t>https://www.destatis.de/DE/Themen/Gesellschaft-Umwelt/Bevoelkerung/Haushalte-Familien/Methoden/mikrozensus-2020.html</t>
+  </si>
+  <si>
+    <t>Indikator 5.1.2: Erwerbsquote, Erwerbstätigenquote und Erwerbslosenanteil nach Zuwanderungsgeschichte</t>
   </si>
   <si>
     <r>
-      <t>Tabelle 5.2.1: Erwerbsquote, Erwerbstätigenquote und Erwerbslosenanteil nach Zuwanderungsgeschichte</t>
+      <t>Tabelle 5.1.2: Erwerbsquote, Erwerbstätigenquote und Erwerbslosenanteil nach Zuwanderungsgeschichte</t>
     </r>
     <r>
       <rPr>
@@ -153,12 +159,6 @@
       </rPr>
       <t>1,4)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">4) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes: </t>
-  </si>
-  <si>
-    <t>https://www.destatis.de/DE/Themen/Gesellschaft-Umwelt/Bevoelkerung/Haushalte-Familien/Methoden/mikrozensus-2020.html</t>
   </si>
 </sst>
 </file>
@@ -435,6 +435,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -448,40 +479,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -801,8 +801,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:S55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:K46"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,22 +823,22 @@
     </row>
     <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M4" s="2"/>
     </row>
@@ -854,126 +854,126 @@
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32" t="s">
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="40"/>
     </row>
     <row r="7" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="29" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29" t="s">
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29" t="s">
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="29" t="s">
+      <c r="O7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="36"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="31"/>
     </row>
     <row r="8" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="37" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="37" t="s">
+      <c r="H8" s="35"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="32" t="s">
+      <c r="L8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="37" t="s">
+      <c r="M8" s="35"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="38" t="s">
+      <c r="P8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="32" t="s">
+      <c r="Q8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="33"/>
+      <c r="R8" s="40"/>
     </row>
     <row r="9" spans="2:19" s="5" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="39"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="39"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="34"/>
       <c r="L9" s="23" t="s">
         <v>11</v>
       </c>
       <c r="M9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="31"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="39"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="34"/>
       <c r="Q9" s="23" t="s">
         <v>11</v>
       </c>
@@ -982,25 +982,25 @@
       </c>
     </row>
     <row r="10" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="33"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="40"/>
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2704,18 +2704,18 @@
       <c r="N43" s="18"/>
     </row>
     <row r="44" spans="2:19" s="19" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
       <c r="N44" s="20"/>
     </row>
     <row r="45" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2734,36 +2734,36 @@
       <c r="N45" s="18"/>
     </row>
     <row r="46" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
     </row>
     <row r="47" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="34"/>
+      <c r="B47" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
     </row>
     <row r="48" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="40" t="s">
-        <v>27</v>
+      <c r="B48" s="25" t="s">
+        <v>25</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
@@ -2860,6 +2860,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="D10:R10"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="Q8:R8"/>
     <mergeCell ref="B47:K47"/>
     <mergeCell ref="B44:K44"/>
     <mergeCell ref="B46:K46"/>
@@ -2873,18 +2885,6 @@
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="D10:R10"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="Q8:R8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B55" r:id="rId1" xr:uid="{378039AC-FEBF-433F-9CA7-5A8047F9398F}"/>

</xml_diff>